<commit_message>
Aks923 commit to new repo
</commit_message>
<xml_diff>
--- a/src/TestData/TestData.xlsx
+++ b/src/TestData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
   <si>
     <t>URL</t>
   </si>
@@ -122,13 +122,280 @@
   </si>
   <si>
     <t>test@test.com</t>
+  </si>
+  <si>
+    <t>WISE Anopup UP title check</t>
+  </si>
+  <si>
+    <t>Choose an experience</t>
+  </si>
+  <si>
+    <t>anuj.kumar.sharma@hp.com</t>
+  </si>
+  <si>
+    <t>If passed in Red font-means its anonymous route</t>
+  </si>
+  <si>
+    <t>c04348351</t>
+  </si>
+  <si>
+    <t>prod doc=c04348351</t>
+  </si>
+  <si>
+    <t>Search result check-Assert</t>
+  </si>
+  <si>
+    <t>DocID search_Prod document[Enter Doc ID]</t>
+  </si>
+  <si>
+    <t>DocID search_Prod document[Assert Text]</t>
+  </si>
+  <si>
+    <t>prod doc=c04348351 title on column 'F'</t>
+  </si>
+  <si>
+    <t>Part of login test-false positive-Fail for CRM flow-pass</t>
+  </si>
+  <si>
+    <t>DocumentRendering_ProductDocument</t>
+  </si>
+  <si>
+    <t>Rating_ProductDocument</t>
+  </si>
+  <si>
+    <t>#6BC039</t>
+  </si>
+  <si>
+    <t>Feedback_ProductDocument</t>
+  </si>
+  <si>
+    <t>Submitted Successfully</t>
+  </si>
+  <si>
+    <t>prod doc=c04348351-use this row for assert and genric text input</t>
+  </si>
+  <si>
+    <t>DocID search_Process document[Enter Doc ID]</t>
+  </si>
+  <si>
+    <t>DocID search_Process document[Assert Text]</t>
+  </si>
+  <si>
+    <t>c01268663</t>
+  </si>
+  <si>
+    <t>Use the Xpath of generic search box &amp; search DOcID div.This is process doc ID</t>
+  </si>
+  <si>
+    <t>Use the Xpath of generic search box &amp; search DOcID div.This is Manual doc ID</t>
+  </si>
+  <si>
+    <t>DocID search_Manual document[Enter Doc ID]</t>
+  </si>
+  <si>
+    <t>DocID search_Manual document[Assert Text]</t>
+  </si>
+  <si>
+    <t>Document rendering_Process Doc[Title]</t>
+  </si>
+  <si>
+    <t>c04110219</t>
+  </si>
+  <si>
+    <t>process doc:c04110219</t>
+  </si>
+  <si>
+    <t>ADF Troubleshooting</t>
+  </si>
+  <si>
+    <t>http://h10032.www1.hp.com/ctg/Manual/c01268663.pdf</t>
+  </si>
+  <si>
+    <t>Manualdoc URL-c01268663</t>
+  </si>
+  <si>
+    <t>Document rendering/open Manual Doc</t>
+  </si>
+  <si>
+    <t>Rating_ProcessDocument</t>
+  </si>
+  <si>
+    <t>URL under constant:URL_ProcessBookmarkDoc</t>
+  </si>
+  <si>
+    <t>Feedback_ProcessDocument</t>
+  </si>
+  <si>
+    <t>c04110219(ujsing prod doc -cases/xpath)</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>INPUT:search by product term e.g pa</t>
+  </si>
+  <si>
+    <t>Search_ByProductTerm_ProdContext_AssertResult</t>
+  </si>
+  <si>
+    <t>HP Stream Notebook - 11-d008tu(K5C54PA)</t>
+  </si>
+  <si>
+    <t>NavigateToPDPPage_SearchTerm</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Object found used:for Image</t>
+  </si>
+  <si>
+    <t>PDP page</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Verify Tools Display</t>
+  </si>
+  <si>
+    <t>UI Experience toggle</t>
+  </si>
+  <si>
+    <t>UI Experience toggle_Assert and click</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Verify UI exp link_found?</t>
+  </si>
+  <si>
+    <t>UI Experience toggle_Assert Selection</t>
+  </si>
+  <si>
+    <t>selected consumer</t>
+  </si>
+  <si>
+    <t>UI Experience toggle_Assert default Selection</t>
+  </si>
+  <si>
+    <t>back to commercial</t>
+  </si>
+  <si>
+    <t>Verify Process Tab display</t>
+  </si>
+  <si>
+    <t>Verify Product Tab display</t>
+  </si>
+  <si>
+    <t>Verify HP logo is displayed</t>
+  </si>
+  <si>
+    <t>any page</t>
+  </si>
+  <si>
+    <t>Verify Privacy link in footer</t>
+  </si>
+  <si>
+    <t>Verify Term Of Use link in footer</t>
+  </si>
+  <si>
+    <t>Verify SIteMap in footer</t>
+  </si>
+  <si>
+    <t>Verify Footer displayed</t>
+  </si>
+  <si>
+    <t>Site Map</t>
+  </si>
+  <si>
+    <t>Terms of Use</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>Verify CopyRight link in footer</t>
+  </si>
+  <si>
+    <t>Footer links</t>
+  </si>
+  <si>
+    <t>Processes</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Use ObjectFound- no text for footer div</t>
+  </si>
+  <si>
+    <t>Copyrights</t>
+  </si>
+  <si>
+    <t>© 2018 Hewlett-Packard Development Company, L.P.</t>
+  </si>
+  <si>
+    <t>Search_ByProductTerm_ProdContext_Able to input search term</t>
+  </si>
+  <si>
+    <t>PDP-TMS_click Product Link status</t>
+  </si>
+  <si>
+    <t>Verify the 2nd Category_top</t>
+  </si>
+  <si>
+    <t>Verify the 3rd Category_top</t>
+  </si>
+  <si>
+    <t>Verify the 4th Category_top</t>
+  </si>
+  <si>
+    <t>HP Printers</t>
+  </si>
+  <si>
+    <t>HP ENVY Printers</t>
+  </si>
+  <si>
+    <t>HP ENVY 100 e-All-in-One Printer series - D410</t>
+  </si>
+  <si>
+    <t>HP ENVY 100 e-All-in-One Printer - D410a</t>
+  </si>
+  <si>
+    <t>CN517A</t>
+  </si>
+  <si>
+    <t>Verify the 5th level_SKU</t>
+  </si>
+  <si>
+    <t>Launch Product Detail Page</t>
+  </si>
+  <si>
+    <t>Launch button found</t>
+  </si>
+  <si>
+    <t>Assert_Verify the first item_HP printer</t>
+  </si>
+  <si>
+    <t>Click_Verify the first item_HP printer</t>
+  </si>
+  <si>
+    <t>sit.hat-07</t>
+  </si>
+  <si>
+    <t>HP DeskJet, ENVY 5540 Printers - Paper Jam Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +419,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +445,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,13 +468,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -492,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,45 +826,45 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -582,10 +873,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>123</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>21</v>
@@ -657,6 +951,393 @@
       </c>
       <c r="F12" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="F48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="F49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -664,8 +1345,9 @@
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="F24" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>